<commit_message>
2021.01.29 영화 목록 점
</commit_message>
<xml_diff>
--- a/영화/영화.xlsx
+++ b/영화/영화.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\book\영화\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8884088-77A6-4E0D-888D-6F70B3C87433}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA94F46F-4BA6-4027-BDB0-F4170AB0B12A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="231">
   <si>
     <t>3번 초콜릿 영상</t>
   </si>
@@ -926,6 +926,211 @@
         <family val="2"/>
       </rPr>
       <t xml:space="preserve"> 2017</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>일본패망하루전 2015</t>
+  </si>
+  <si>
+    <t>보이지 않는 목격자 2019</t>
+  </si>
+  <si>
+    <t>내일 세상의 종말이 올지라도 2019</t>
+  </si>
+  <si>
+    <t>솔리스 2018</t>
+  </si>
+  <si>
+    <t>살인귀를 키우는 여자 2019</t>
+  </si>
+  <si>
+    <t>디파티드 2006(더빙)</t>
+  </si>
+  <si>
+    <t>미스터 노바디 2009</t>
+  </si>
+  <si>
+    <t>변방의 형제들 2019</t>
+  </si>
+  <si>
+    <t>충격과 공포 2017</t>
+  </si>
+  <si>
+    <t>해변의 여인 2006</t>
+  </si>
+  <si>
+    <t>더 도어 2009(더빙)</t>
+  </si>
+  <si>
+    <t>타인의 취향 2000</t>
+  </si>
+  <si>
+    <t>황금화 엄마의 일기 2017</t>
+  </si>
+  <si>
+    <t>공범 2012</t>
+  </si>
+  <si>
+    <t>스턱 인 러브 2012</t>
+  </si>
+  <si>
+    <t>스턱 2017</t>
+  </si>
+  <si>
+    <t>스마일 페이스 킬러 2020</t>
+  </si>
+  <si>
+    <t>진가미후왕 대성무쌍 2020</t>
+  </si>
+  <si>
+    <t>금의위 3인의 무사 2020</t>
+  </si>
+  <si>
+    <t>모든 걸 걸었어 2020</t>
+  </si>
+  <si>
+    <t>인랜드 엠파이어 2006</t>
+  </si>
+  <si>
+    <t>어 밀리언 리틀 피시즈 2018</t>
+  </si>
+  <si>
+    <t>리뎀션 데이 2021</t>
+  </si>
+  <si>
+    <t>천사는 바이러스 2021</t>
+  </si>
+  <si>
+    <t>바이크 원정대 인 이탈리아 2020</t>
+  </si>
+  <si>
+    <t>썸머 85 2020</t>
+  </si>
+  <si>
+    <t>도쿄 소나타 2008</t>
+  </si>
+  <si>
+    <t>순천부 살인가면 2019</t>
+  </si>
+  <si>
+    <t>일본</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>영국</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>한국</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>밀정</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> 1930 2017</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>홍콩</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>다운</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>각오는</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>됐나</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>거기</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>여자</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> 2018</t>
     </r>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -1326,11 +1531,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L178"/>
+  <dimension ref="A1:L219"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A155" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B147" sqref="B147"/>
+      <pane ySplit="1" topLeftCell="A197" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D182" sqref="D182"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -2304,13 +2509,248 @@
         <v>190</v>
       </c>
     </row>
-    <row r="177" spans="2:2">
+    <row r="177" spans="1:4">
       <c r="B177" s="2" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="178" spans="2:2">
+    <row r="178" spans="1:4">
+      <c r="A178" s="6">
+        <v>44225</v>
+      </c>
       <c r="B178" s="7"/>
+    </row>
+    <row r="179" spans="1:4">
+      <c r="B179" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="180" spans="1:4">
+      <c r="B180" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="D180" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="181" spans="1:4">
+      <c r="B181" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="C181" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="182" spans="1:4">
+      <c r="B182" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="C182" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="183" spans="1:4">
+      <c r="B183" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="C183" t="s">
+        <v>225</v>
+      </c>
+      <c r="D183" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="184" spans="1:4">
+      <c r="B184" s="2" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="185" spans="1:4">
+      <c r="B185" s="2" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="186" spans="1:4">
+      <c r="B186" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="187" spans="1:4">
+      <c r="B187" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="188" spans="1:4">
+      <c r="B188" s="2" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="189" spans="1:4">
+      <c r="B189" s="2" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="190" spans="1:4">
+      <c r="B190" s="2" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="191" spans="1:4">
+      <c r="B191" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="C191" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="192" spans="1:4">
+      <c r="B192" s="2" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="193" spans="2:4">
+      <c r="B193" s="2" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="194" spans="2:4">
+      <c r="B194" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="195" spans="2:4">
+      <c r="B195" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="196" spans="2:4">
+      <c r="B196" s="2" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="197" spans="2:4">
+      <c r="B197" s="8" t="s">
+        <v>227</v>
+      </c>
+      <c r="C197" t="s">
+        <v>228</v>
+      </c>
+      <c r="D197" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="198" spans="2:4">
+      <c r="B198" s="2" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="199" spans="2:4">
+      <c r="B199" s="2" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="200" spans="2:4">
+      <c r="B200" s="2" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="201" spans="2:4">
+      <c r="B201" s="8" t="s">
+        <v>230</v>
+      </c>
+      <c r="C201" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="202" spans="2:4">
+      <c r="B202" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="203" spans="2:4">
+      <c r="B203" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="204" spans="2:4">
+      <c r="B204" s="2" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="205" spans="2:4">
+      <c r="B205" s="2" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="206" spans="2:4">
+      <c r="B206" s="2" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="207" spans="2:4">
+      <c r="B207" s="2" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="208" spans="2:4">
+      <c r="B208" s="2" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="209" spans="2:2">
+      <c r="B209" s="2" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="210" spans="2:2">
+      <c r="B210" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="211" spans="2:2">
+      <c r="B211" s="2" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="212" spans="2:2">
+      <c r="B212" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="213" spans="2:2">
+      <c r="B213" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="214" spans="2:2">
+      <c r="B214" s="2" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="215" spans="2:2">
+      <c r="B215" s="2" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="216" spans="2:2">
+      <c r="B216" s="2" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="217" spans="2:2">
+      <c r="B217" s="2" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="218" spans="2:2">
+      <c r="B218" s="2" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="219" spans="2:2">
+      <c r="B219" s="2" t="s">
+        <v>223</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>

</xml_diff>